<commit_message>
Remove mentions to Matlab
</commit_message>
<xml_diff>
--- a/templates/reliability_data.xlsx
+++ b/templates/reliability_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.barla\Documents\Local_codes\HVDCWISE_TEA.jl\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC3237-A6EC-470E-BC41-475C9215C43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1361FF-3B1B-4925-BE01-A7C98B991EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="360" windowWidth="19110" windowHeight="10035" xr2:uid="{C57834E6-C588-4116-B15D-7ADB3B8705E5}"/>
   </bookViews>
@@ -101,23 +101,30 @@
     <t>Correlation between poles</t>
   </si>
   <si>
-    <t>0: no correlation. 1: perfect correlation</t>
-  </si>
-  <si>
     <t>Number between 0 &amp; 1</t>
   </si>
   <si>
     <t>MTTR</t>
+  </si>
+  <si>
+    <t>0: no correlation. 1: perfect correlation /!\ Feature not implement in the current version (0 is mandatory)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +497,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +513,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -537,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,8 +564,8 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,6 +674,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
+    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100360305CF8A5F8A4B86568FB88F41EB51" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7820bdd98b12bbce6701f392baa49827">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xmlns:ns3="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a7208ee71179b2cd86960a83168177e" ns2:_="" ns3:_="">
     <xsd:import namespace="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
@@ -906,18 +926,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576" xsi:nil="true"/>
-    <TaxCatchAll xmlns="e2fe3da4-e7b1-4e71-a513-56b717f56f6b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -928,6 +936,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F92369D0-E2D9-438E-977C-26874210B002}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
+    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E7CE95-6C7D-4EA1-9372-E88699DF4BE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -946,17 +965,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F92369D0-E2D9-438E-977C-26874210B002}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37bcdbbe-1b84-46f8-a2e4-bedf5bd24576"/>
-    <ds:schemaRef ds:uri="e2fe3da4-e7b1-4e71-a513-56b717f56f6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB8192F-3B07-4D72-B166-5C843A05F0AB}">
   <ds:schemaRefs>

</xml_diff>